<commit_message>
tried to use RAFs. did not work
</commit_message>
<xml_diff>
--- a/init/initialization.xlsx
+++ b/init/initialization.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -47,22 +47,28 @@
     <t>I_Supplier.xml</t>
   </si>
   <si>
+    <t>Feb 17, 2022 (02:54:36 EST)</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>I_Plant.xml</t>
+  </si>
+  <si>
+    <t>Feb 17, 2022 (02:54:40 EST)</t>
+  </si>
+  <si>
+    <t>Solicitation</t>
+  </si>
+  <si>
+    <t>I_Solicitation.xml</t>
+  </si>
+  <si>
     <t>Feb 29, 2004 (12:00:00 EST)</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>I_Plant.xml</t>
-  </si>
-  <si>
-    <t>Solicitation</t>
-  </si>
-  <si>
-    <t>I_Solicitation.xml</t>
   </si>
   <si>
     <t>BOM</t>
@@ -197,7 +203,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -208,7 +214,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -217,10 +223,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -231,7 +237,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -240,10 +246,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -254,19 +260,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -277,19 +283,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -303,7 +309,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -312,7 +318,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -326,7 +332,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -335,7 +341,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -346,19 +352,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
@@ -369,19 +375,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -392,19 +398,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -415,19 +421,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
A lot of work on importing from file to db
</commit_message>
<xml_diff>
--- a/init/initialization.xlsx
+++ b/init/initialization.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -35,58 +35,67 @@
     <t>Status</t>
   </si>
   <si>
+    <t>SupplierDumb</t>
+  </si>
+  <si>
+    <t>DRX</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>I_Supplier.xml</t>
+  </si>
+  <si>
+    <t>Feb 18, 2022 (11:16:32 EST)</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>DRXX</t>
+  </si>
+  <si>
+    <t>I_Plant.xml</t>
+  </si>
+  <si>
+    <t>Feb 18, 2022 (11:14:55 EST)</t>
+  </si>
+  <si>
+    <t>Solicitation</t>
+  </si>
+  <si>
+    <t>I_Solicitation.xml</t>
+  </si>
+  <si>
+    <t>Feb 18, 2022 (11:16:05 EST)</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>I_BOM.xml</t>
+  </si>
+  <si>
+    <t>Feb 29, 2004 (12:00:00 EST)</t>
+  </si>
+  <si>
+    <t>RequestFile</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>E_RequestFile.xml</t>
+  </si>
+  <si>
+    <t>E_BOM.xml</t>
+  </si>
+  <si>
     <t>Supplier</t>
-  </si>
-  <si>
-    <t>DRX</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>I_Supplier.xml</t>
-  </si>
-  <si>
-    <t>Feb 17, 2022 (02:54:36 EST)</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>I_Plant.xml</t>
-  </si>
-  <si>
-    <t>Feb 17, 2022 (02:54:40 EST)</t>
-  </si>
-  <si>
-    <t>Solicitation</t>
-  </si>
-  <si>
-    <t>I_Solicitation.xml</t>
-  </si>
-  <si>
-    <t>Feb 29, 2004 (12:00:00 EST)</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>I_BOM.xml</t>
-  </si>
-  <si>
-    <t>RequestFile</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>E_RequestFile.xml</t>
-  </si>
-  <si>
-    <t>E_BOM.xml</t>
   </si>
   <si>
     <t>GYU</t>
@@ -194,16 +203,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -214,7 +223,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -223,10 +232,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -237,7 +246,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -246,10 +255,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -260,19 +269,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -283,19 +292,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -306,10 +315,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -318,7 +327,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>
@@ -332,16 +341,16 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -352,19 +361,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
         <v>12</v>
@@ -375,19 +384,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
@@ -398,19 +407,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
@@ -421,19 +430,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
         <v>12</v>

</xml_diff>